<commit_message>
collecting data on FSR_S2 - second round
</commit_message>
<xml_diff>
--- a/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
+++ b/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr19556\Desktop\FSR_AppliedMedical-main\FSR_AppliedMedical-main\data\FSR_S2\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S2/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F1550-607B-48E9-B903-C670764AD2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCC2AE5-7B13-8F46-8772-6232E9AACA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="11520" yWindow="880" windowWidth="20100" windowHeight="13800" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>FSR</t>
   </si>
@@ -62,19 +62,22 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Pre-Cond</t>
-  </si>
-  <si>
-    <t>Post-Cond</t>
-  </si>
-  <si>
     <t>Event</t>
   </si>
   <si>
     <t>FSR_S2</t>
   </si>
   <si>
-    <t>152.65029.</t>
+    <t>Pre-Cond - 1</t>
+  </si>
+  <si>
+    <t>Post-Cond - 1</t>
+  </si>
+  <si>
+    <t>Pre-Cond - 2</t>
+  </si>
+  <si>
+    <t>Post-Cond - 2</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -128,6 +131,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -147,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,22 +452,22 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="3"/>
-    <col min="2" max="2" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="3"/>
     <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" style="3"/>
+    <col min="7" max="7" width="8.83203125" style="3"/>
     <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.77734375" style="3"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -484,59 +490,81 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
+        <v>21806.880949999999</v>
+      </c>
+      <c r="C2" s="4">
+        <v>152.65029000000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-1.0078400000000001</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3.82E-3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.99185999999999996</v>
+      </c>
+      <c r="G2" s="4">
+        <v>7594.8168100000003</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>16350.468129999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>95.634039999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-0.88514999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3.16E-3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.99846999999999997</v>
+      </c>
+      <c r="G3" s="4">
+        <v>9592.5557100000005</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
-        <v>21806.880949999999</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1">
-        <v>-1.0078400000000001</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3.82E-3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.99185999999999996</v>
-      </c>
-      <c r="G2" s="1">
-        <v>7594.8168100000003</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>16350.468129999999</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-0.88514999999999999</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.99846999999999997</v>
-      </c>
-      <c r="G3" s="1">
-        <v>9592.5557100000005</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -546,7 +574,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>

<commit_message>
calibration comparison data S2 swag
</commit_message>
<xml_diff>
--- a/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
+++ b/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S2/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCC2AE5-7B13-8F46-8772-6232E9AACA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB79FF2-927A-B543-8B6C-91F991F160A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="880" windowWidth="20100" windowHeight="13800" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="-580" yWindow="2220" windowWidth="16640" windowHeight="13800" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -552,6 +552,24 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="1">
+        <v>26459.371500000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>119.01181</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1.0608299999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.47E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7901.9475499999999</v>
+      </c>
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
@@ -559,6 +577,24 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21939.003530000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>245.64123000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-0.99304999999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.96469000000000005</v>
+      </c>
+      <c r="G5" s="1">
+        <v>42048.431120000001</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
finished most of the data analysis for FSR_02
</commit_message>
<xml_diff>
--- a/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
+++ b/data/FSR_S2/calibration/FSR_S2 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S2/calibration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S2/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB79FF2-927A-B543-8B6C-91F991F160A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{9EB79FF2-927A-B543-8B6C-91F991F160A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF47E836-8C22-413F-8439-1F23A1DE2D14}"/>
   <bookViews>
-    <workbookView xWindow="-580" yWindow="2220" windowWidth="16640" windowHeight="13800" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="1710" yWindow="2865" windowWidth="21600" windowHeight="12735" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>FSR</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Post-Cond - 2</t>
+  </si>
+  <si>
+    <t>Applies to Stability 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Post-Stability - 2</t>
+  </si>
+  <si>
+    <t>Post-Stability - 3</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -134,6 +143,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -153,9 +165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +205,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +311,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,22 +464,23 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="3"/>
     <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="3"/>
-    <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -522,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -548,7 +561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -573,8 +586,11 @@
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -599,18 +615,63 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>24152.816739999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>117.35845</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1.08121</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.6700000000000001E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6944.35635</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <v>19782.556499999999</v>
+      </c>
+      <c r="C7" s="5">
+        <v>98.389030000000005</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-0.9879</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2.7100000000000002E-3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.99973000000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <v>6923.6917100000001</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>